<commit_message>
Ajuste para seleccionar la fecha
</commit_message>
<xml_diff>
--- a/RetoSQAScreenplay/data/DatosSanAngel.xlsx
+++ b/RetoSQAScreenplay/data/DatosSanAngel.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C38C4CF-2423-40C6-AC7B-1993156B02EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="12820"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compras" sheetId="1" r:id="rId1"/>
@@ -125,25 +126,25 @@
     <t>Carlos</t>
   </si>
   <si>
-    <t>Ariza</t>
-  </si>
-  <si>
-    <t>carlitos@hotmail.com</t>
-  </si>
-  <si>
-    <t>Bertilde sosa</t>
-  </si>
-  <si>
-    <t>Cll 5ta</t>
-  </si>
-  <si>
-    <t>Edificio</t>
-  </si>
-  <si>
-    <t>Para ti</t>
-  </si>
-  <si>
-    <t>CAR</t>
+    <t>Alfred</t>
+  </si>
+  <si>
+    <t>car@gmail.com</t>
+  </si>
+  <si>
+    <t>Marina Sosa</t>
+  </si>
+  <si>
+    <t>Cll 45 - 78</t>
+  </si>
+  <si>
+    <t>Apto</t>
+  </si>
+  <si>
+    <t>Cariño</t>
+  </si>
+  <si>
+    <t>CAAS</t>
   </si>
   <si>
     <t>Prueba2</t>
@@ -152,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,9 +254,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -293,9 +294,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,7 +331,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -365,7 +366,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -538,11 +539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,8 +553,9 @@
     <col min="3" max="3" width="17.81640625" customWidth="1"/>
     <col min="4" max="4" width="12.453125" customWidth="1"/>
     <col min="5" max="5" width="10.453125" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.453125" customWidth="1"/>
-    <col min="12" max="12" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.26953125" customWidth="1"/>
     <col min="18" max="18" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -664,7 +666,7 @@
         <v>19</v>
       </c>
       <c r="Q2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R2">
         <v>3214785965</v>
@@ -684,10 +686,10 @@
         <v>36</v>
       </c>
       <c r="E3">
-        <v>654321</v>
+        <v>987654</v>
       </c>
       <c r="F3">
-        <v>32189754</v>
+        <v>3117889652</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>37</v>
@@ -696,7 +698,7 @@
         <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J3" t="s">
         <v>39</v>
@@ -705,7 +707,7 @@
         <v>40</v>
       </c>
       <c r="L3">
-        <v>325785212</v>
+        <v>3568795641</v>
       </c>
       <c r="M3" t="s">
         <v>41</v>
@@ -720,31 +722,31 @@
         <v>43</v>
       </c>
       <c r="Q3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="R3">
-        <v>3134007885</v>
+        <v>3247896321</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2" location="/"/>
-    <hyperlink ref="G3" r:id="rId3"/>
-    <hyperlink ref="A3" r:id="rId4" location="/"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" location="/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G3" r:id="rId3" xr:uid="{F3C2AB4B-9064-44BF-901E-0D4D8FB7EE4C}"/>
+    <hyperlink ref="A3" r:id="rId4" location="/" xr:uid="{4177F1F6-23BA-4028-89DD-BE1CB1B8BDBD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Data!$A$2:$A$7</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Data!$C$2:$C$3</xm:f>
           </x14:formula1>
@@ -757,7 +759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>